<commit_message>
Adding code for Adaptive algorithm
</commit_message>
<xml_diff>
--- a/Runtime_Latency_values.xlsx
+++ b/Runtime_Latency_values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="-220" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,11 +273,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2118329712"/>
-        <c:axId val="-2122159072"/>
+        <c:axId val="2087545008"/>
+        <c:axId val="2084712464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2118329712"/>
+        <c:axId val="2087545008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,12 +390,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122159072"/>
+        <c:crossAx val="2084712464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122159072"/>
+        <c:axId val="2084712464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,7 +513,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118329712"/>
+        <c:crossAx val="2087545008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1416,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1480,6 +1480,14 @@
         <v>3.1349999999999998</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>1.5309999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>